<commit_message>
Cambios necesarios en ROL y MENU
</commit_message>
<xml_diff>
--- a/database/seeds/Catalogos/Menu.xlsx
+++ b/database/seeds/Catalogos/Menu.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
-  <si>
-    <t>Administracion</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="81">
   <si>
     <t>#</t>
   </si>
@@ -38,9 +35,6 @@
     <t>cog</t>
   </si>
   <si>
-    <t>Categorias</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>truck</t>
   </si>
   <si>
-    <t>Gestionar Pedido</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>Serie</t>
   </si>
   <si>
-    <t>Lista facturas</t>
-  </si>
-  <si>
     <t>Transporte</t>
   </si>
   <si>
@@ -224,9 +212,6 @@
     <t>Transport</t>
   </si>
   <si>
-    <t>Transporte Histórico</t>
-  </si>
-  <si>
     <t>transport/history</t>
   </si>
   <si>
@@ -246,19 +231,66 @@
   </si>
   <si>
     <t>Vehicle</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>Administración</t>
+  </si>
+  <si>
+    <t>Catégorias</t>
+  </si>
+  <si>
+    <t>Gestionar pedido</t>
+  </si>
+  <si>
+    <t>Facturas realizadas</t>
+  </si>
+  <si>
+    <t>Transporte histórico</t>
+  </si>
+  <si>
+    <t>gerente</t>
+  </si>
+  <si>
+    <t>bodega</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>comprar</t>
+  </si>
+  <si>
+    <t>facturador</t>
+  </si>
+  <si>
+    <t>repartidor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -281,8 +313,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,732 +612,772 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C14" t="s">
         <v>55</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D16">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>25</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
       </c>
       <c r="D18">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19">
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Menu sugerido create, update, delete
</commit_message>
<xml_diff>
--- a/database/seeds/Catalogos/Menu.xlsx
+++ b/database/seeds/Catalogos/Menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="118">
   <si>
     <t>#</t>
   </si>
@@ -77,12 +77,6 @@
     <t>Provider</t>
   </si>
   <si>
-    <t>Productos faltantes</t>
-  </si>
-  <si>
-    <t>MissingProduct</t>
-  </si>
-  <si>
     <t>Compras</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>provider</t>
   </si>
   <si>
-    <t>missing_product</t>
-  </si>
-  <si>
     <t>rol</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>Administración</t>
   </si>
   <si>
-    <t>Catégorias</t>
-  </si>
-  <si>
     <t>Gestionar pedido</t>
   </si>
   <si>
@@ -267,6 +255,129 @@
   </si>
   <si>
     <t>Person</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>purchase_create</t>
+  </si>
+  <si>
+    <t>PurchaseCreate</t>
+  </si>
+  <si>
+    <t>purchase_view_info</t>
+  </si>
+  <si>
+    <t>PurchaseViewInfo</t>
+  </si>
+  <si>
+    <t>school_balance</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Asignar pedido</t>
+  </si>
+  <si>
+    <t>assign_product</t>
+  </si>
+  <si>
+    <t>AssignProduct</t>
+  </si>
+  <si>
+    <t>Transporte Check</t>
+  </si>
+  <si>
+    <t>transport/check</t>
+  </si>
+  <si>
+    <t>TransportCheck</t>
+  </si>
+  <si>
+    <t>Escuela balance</t>
+  </si>
+  <si>
+    <t>Compra listado</t>
+  </si>
+  <si>
+    <t>Compra nueva</t>
+  </si>
+  <si>
+    <t>Balance nuevo</t>
+  </si>
+  <si>
+    <t>school_create_balance</t>
+  </si>
+  <si>
+    <t>CreateBalance</t>
+  </si>
+  <si>
+    <t>invoice_create</t>
+  </si>
+  <si>
+    <t>Factura crear</t>
+  </si>
+  <si>
+    <t>InvoiceCreate</t>
+  </si>
+  <si>
+    <t>invoice_download</t>
+  </si>
+  <si>
+    <t>Factura descargar</t>
+  </si>
+  <si>
+    <t>InvoiceDownload</t>
+  </si>
+  <si>
+    <t>new/school</t>
+  </si>
+  <si>
+    <t>NewSchool</t>
+  </si>
+  <si>
+    <t>Escuela nueva</t>
+  </si>
+  <si>
+    <t>information/school</t>
+  </si>
+  <si>
+    <t>Escuela información</t>
+  </si>
+  <si>
+    <t>InformationSchool</t>
+  </si>
+  <si>
+    <t>Menú</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>MenuSugge</t>
+  </si>
+  <si>
+    <t>new/menu</t>
+  </si>
+  <si>
+    <t>Menú Nuevo</t>
+  </si>
+  <si>
+    <t>NewMenu</t>
+  </si>
+  <si>
+    <t>edit/menu</t>
+  </si>
+  <si>
+    <t>EditMenu</t>
+  </si>
+  <si>
+    <t>Menú Editar</t>
   </si>
 </sst>
 </file>
@@ -599,17 +710,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
@@ -619,7 +730,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -637,24 +748,24 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -669,16 +780,16 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -686,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -701,13 +812,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -715,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -730,16 +841,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -747,7 +858,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -762,16 +873,16 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -779,7 +890,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -794,13 +905,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -823,16 +934,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -840,7 +951,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -855,27 +966,27 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -887,27 +998,27 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -919,59 +1030,59 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -983,56 +1094,56 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -1044,24 +1155,24 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>13</v>
@@ -1073,27 +1184,27 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16">
         <v>13</v>
@@ -1105,50 +1216,50 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>23</v>
-      </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1160,24 +1271,24 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D19">
         <v>17</v>
@@ -1189,24 +1300,24 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -1218,24 +1329,24 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D21">
         <v>11</v>
@@ -1247,10 +1358,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1264,7 +1375,7 @@
         <v>45</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -1273,27 +1384,21 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>11</v>
@@ -1305,24 +1410,30 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -1331,53 +1442,414 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" t="s">
+        <v>70</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" t="s">
+        <v>70</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" t="s">
+        <v>70</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38" t="s">
+        <v>70</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>